<commit_message>
Feat lifespan error management
</commit_message>
<xml_diff>
--- a/excel-files/ean/ean_codes.xlsx
+++ b/excel-files/ean/ean_codes.xlsx
@@ -443,28 +443,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>6680489841198</t>
+          <t>5171429829879</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2607352459873</t>
+          <t>4715172468769</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>5447221072876</t>
+          <t>2483774646197</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>5543951941740</t>
+          <t>5297607499672</t>
         </is>
       </c>
     </row>

</xml_diff>